<commit_message>
Updated the previous code
</commit_message>
<xml_diff>
--- a/AutomationFramework/Data sheet/Forgot_Pass_Sheet.xlsx
+++ b/AutomationFramework/Data sheet/Forgot_Pass_Sheet.xlsx
@@ -130,9 +130,6 @@
     <t>drop_down</t>
   </si>
   <si>
-    <t>logout</t>
-  </si>
-  <si>
     <t>browser_back_option</t>
   </si>
   <si>
@@ -148,18 +145,12 @@
     <t>//*[@id="header-icon-3"]</t>
   </si>
   <si>
-    <t>//*[@id="header-icon-0"]</t>
-  </si>
-  <si>
     <t>//*[@id="header-icon-1"]</t>
   </si>
   <si>
     <t>//*[@id="header-icon-2"]</t>
   </si>
   <si>
-    <t>//*[@id="side-nav-pane-items"]/div/button[1]/span[1]</t>
-  </si>
-  <si>
     <t>//*[@id="root"]/div/div[3]/div[2]/div/div/div/div[2]/div[2]/div/div/button</t>
   </si>
   <si>
@@ -196,61 +187,70 @@
     <t>//button[@id='login']</t>
   </si>
   <si>
+    <t>side_arrow</t>
+  </si>
+  <si>
+    <t>//body/div[@id='root']/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/img[1]</t>
+  </si>
+  <si>
+    <t>/html/body/form/div/div[2]/div[4]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>plus_one</t>
+  </si>
+  <si>
+    <t>forgot_password_link</t>
+  </si>
+  <si>
+    <t>//a[@id='forgot-password']</t>
+  </si>
+  <si>
+    <t>signup_first_name</t>
+  </si>
+  <si>
+    <t>//input[@id='first-name-field']</t>
+  </si>
+  <si>
+    <t>//input[@id='inputUsername']</t>
+  </si>
+  <si>
+    <t>//input[@id='inputPassword']</t>
+  </si>
+  <si>
+    <t>forgot_password_title</t>
+  </si>
+  <si>
+    <t>//div[@id='page-container']/h2</t>
+  </si>
+  <si>
+    <t>logout1</t>
+  </si>
+  <si>
+    <t>//body/div[@id='root']/div[1]/div[2]/div[1]/div[1]/button[1]</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>2223330909</t>
+  </si>
+  <si>
+    <t>Carol@12345</t>
+  </si>
+  <si>
     <t>//span[contains(text(),'Utilities')]</t>
   </si>
   <si>
-    <t>side_arrow</t>
-  </si>
-  <si>
-    <t>//body/div[@id='root']/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/img[1]</t>
-  </si>
-  <si>
-    <t>//body/div[@id='root']/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/div[1]/div[3]/span[1]/div[1]</t>
-  </si>
-  <si>
-    <t>/html/body/form/div/div[2]/div[4]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>plus_one</t>
-  </si>
-  <si>
-    <t>forgot_password_link</t>
-  </si>
-  <si>
-    <t>//a[@id='forgot-password']</t>
-  </si>
-  <si>
-    <t>signup_first_name</t>
-  </si>
-  <si>
-    <t>//input[@id='first-name-field']</t>
-  </si>
-  <si>
-    <t>//input[@id='inputUsername']</t>
-  </si>
-  <si>
-    <t>//input[@id='inputPassword']</t>
-  </si>
-  <si>
-    <t>forgot_password_title</t>
-  </si>
-  <si>
-    <t>//div[@id='page-container']/h2</t>
-  </si>
-  <si>
-    <t>logout1</t>
-  </si>
-  <si>
-    <t>//body/div[@id='root']/div[1]/div[2]/div[1]/div[1]/button[1]</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>2223330909</t>
-  </si>
-  <si>
-    <t>Carol@12345</t>
+    <t>logout_home</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/img[1]</t>
+  </si>
+  <si>
+    <t>//body/div[@id='root']/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/span[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Home')]</t>
   </si>
 </sst>
 </file>
@@ -655,26 +655,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -693,15 +693,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.26953125" customWidth="1"/>
     <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="78" customWidth="1"/>
+    <col min="3" max="3" width="82.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -734,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -764,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -786,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -797,7 +797,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -841,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -852,23 +852,23 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -876,18 +876,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -904,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -915,110 +915,111 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
all the home page positive scenario
</commit_message>
<xml_diff>
--- a/AutomationFramework/Data sheet/Forgot_Pass_Sheet.xlsx
+++ b/AutomationFramework/Data sheet/Forgot_Pass_Sheet.xlsx
@@ -11,13 +11,15 @@
     <sheet name="Object_Locator" sheetId="5" r:id="rId2"/>
     <sheet name="Object Locator1" sheetId="2" r:id="rId3"/>
     <sheet name="Object Locator" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
   <si>
     <t>Field_name</t>
   </si>
@@ -115,12 +117,6 @@
     <t>award_points</t>
   </si>
   <si>
-    <t>second_opinions</t>
-  </si>
-  <si>
-    <t>refer_a_friend</t>
-  </si>
-  <si>
     <t>help</t>
   </si>
   <si>
@@ -133,39 +129,9 @@
     <t>browser_back_option</t>
   </si>
   <si>
-    <t>//*[@id="root"]/div/div[3]/div[2]/div/div/div/div[1]/div[2]/span/div</t>
-  </si>
-  <si>
-    <t>//*[@id="root"]/div/div[3]/div[2]/div/div/div/div[1]/div[3]/span/div</t>
-  </si>
-  <si>
-    <t>//*[@id="root"]/div/div[3]/div[2]/div/div/div/div[1]/div[1]/span/div</t>
-  </si>
-  <si>
-    <t>//*[@id="header-icon-3"]</t>
-  </si>
-  <si>
-    <t>//*[@id="header-icon-1"]</t>
-  </si>
-  <si>
-    <t>//*[@id="header-icon-2"]</t>
-  </si>
-  <si>
-    <t>//*[@id="root"]/div/div[3]/div[2]/div/div/div/div[2]/div[2]/div/div/button</t>
-  </si>
-  <si>
     <t>request_a_second_oponion</t>
   </si>
   <si>
-    <t>//*[@id="root"]/div/div[3]/div[2]/div/div/div/div[2]/div[1]/div/div/button</t>
-  </si>
-  <si>
-    <t>//*[@id="side-nav-pane-items"]/div/button[2]/span[1]/span</t>
-  </si>
-  <si>
-    <t>//*[@id="side-nav-pane-items"]/div/button[3]/span[1]/span</t>
-  </si>
-  <si>
     <t>//*[@id="side-nav-pane-items"]/div/button[4]/span[1]/span</t>
   </si>
   <si>
@@ -244,20 +210,191 @@
     <t>logout_home</t>
   </si>
   <si>
-    <t>//body[1]/div[1]/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/img[1]</t>
-  </si>
-  <si>
-    <t>//body/div[@id='root']/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/span[1]/div[1]</t>
-  </si>
-  <si>
     <t>//span[contains(text(),'Home')]</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[3]/div[2]/div[1]/div[2]/div[2]/div[1]/div[2]/span[1]/div[1]</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Services')]</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Circles')]</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[3]/div[2]/div[1]/div[1]/div[2]/div[1]/div[1]/div[1]/div[1]/div[1]/div[1]/h4[1]</t>
+  </si>
+  <si>
+    <t>bills_title</t>
+  </si>
+  <si>
+    <t>side_arrow_bills</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[3]/div[2]/div[1]/div[1]/div[1]/h3[1]</t>
+  </si>
+  <si>
+    <t>help_msg</t>
+  </si>
+  <si>
+    <t>//div[@class='jss1085']/div/div/div/div/div/h4</t>
+  </si>
+  <si>
+    <t>arrow_wallet</t>
+  </si>
+  <si>
+    <t>//div[@class='jss785']/img</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Wallet')]</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Bills')]</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Manage payments')]</t>
+  </si>
+  <si>
+    <t>wallet_page</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Bills')]</t>
+  </si>
+  <si>
+    <t>bills_page</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Award points')]</t>
+  </si>
+  <si>
+    <t>award_points_page</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Award Points')]</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Second Opinion')]</t>
+  </si>
+  <si>
+    <t>second_opinion_button_page</t>
+  </si>
+  <si>
+    <t>refer_a_friend_page</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Refer a friend')]</t>
+  </si>
+  <si>
+    <t>//button/span[contains(text(),'Request a Second Opinion')]</t>
+  </si>
+  <si>
+    <t>//button/span[contains(text(),'Refer a Friend')]</t>
+  </si>
+  <si>
+    <t>second_opinions_button</t>
+  </si>
+  <si>
+    <t>refer_a_friend_button</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Frequently asked questions')]</t>
+  </si>
+  <si>
+    <t>help_page</t>
+  </si>
+  <si>
+    <t>logout_page</t>
+  </si>
+  <si>
+    <t>//div/h2[contains(text(),'It')]</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Your alerts')]</t>
+  </si>
+  <si>
+    <t>your_alerts_page</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Your profile')]</t>
+  </si>
+  <si>
+    <t>your_profile_tap</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Your profile')]</t>
+  </si>
+  <si>
+    <t>your_profile_page</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Your ratings')]</t>
+  </si>
+  <si>
+    <t>your_rating_page</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[2]/div[1]/div[4]/div[1]/img[1]</t>
+  </si>
+  <si>
+    <t>//div/h3[contains(text(),'Welcome Back')]</t>
+  </si>
+  <si>
+    <t>navigate_back</t>
+  </si>
+  <si>
+    <t>//div/div/div/div/img</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[2]/div[1]/div[3]/div[1]/span[1]/img[1]</t>
+  </si>
+  <si>
+    <t>//body[1]/div[1]/div[1]/div[2]/div[1]/div[2]/div[1]/img[1]</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Your ratings')]</t>
+  </si>
+  <si>
+    <t>your_rating</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Feedback')]</t>
+  </si>
+  <si>
+    <t>feedback</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Contact us')]</t>
+  </si>
+  <si>
+    <t>contact_us</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Privacy Policy')]</t>
+  </si>
+  <si>
+    <t>//div/p[contains(text(),'Terms &amp; Conditions')]</t>
+  </si>
+  <si>
+    <t>privacy_policy</t>
+  </si>
+  <si>
+    <t>terms_conditions</t>
+  </si>
+  <si>
+    <t>class="jss171"</t>
+  </si>
+  <si>
+    <t>//div[@class='jss171']//div//div//div/p</t>
+  </si>
+  <si>
+    <t>common_one</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +430,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FFD5D5D5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -315,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -339,6 +482,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -644,7 +788,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,26 +799,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -691,17 +835,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.26953125" customWidth="1"/>
     <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="82.81640625" customWidth="1"/>
+    <col min="3" max="3" width="87.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -723,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -734,7 +878,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -745,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -755,6 +899,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -764,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -775,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -786,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -796,79 +943,79 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>38</v>
+      <c r="C9" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -876,18 +1023,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -904,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -915,106 +1062,353 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="19" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="409.6" x14ac:dyDescent="0.35">
+      <c r="C55" s="23" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1028,7 +1422,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1203,4 +1597,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="94.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>